<commit_message>
Updating grades with ranks
</commit_message>
<xml_diff>
--- a/notes/PrePublication_Notes.xlsx
+++ b/notes/PrePublication_Notes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t xml:space="preserve">NOM</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Appréciation</t>
   </si>
   <si>
+    <t xml:space="preserve">Rang</t>
+  </si>
+  <si>
     <t xml:space="preserve">A++ : 20</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
     <t xml:space="preserve">Notes &lt; 6</t>
   </si>
   <si>
+    <t xml:space="preserve">Notes = 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nb Etd</t>
   </si>
   <si>
@@ -101,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">% Notes &lt; 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Notes = 0</t>
   </si>
 </sst>
 </file>
@@ -467,13 +476,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ71"/>
+  <dimension ref="A1:AMJ73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.43"/>
@@ -497,7 +506,9 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AMH1" s="0"/>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
@@ -512,8 +523,12 @@
         <f aca="false">IF(D2=20,"A++",IF(D2&gt;=15,"A",IF(D2&gt;=12,"B",IF(D2&gt;=8,"C",IF(D2&gt;=6,"D","E")))))</f>
         <v>C</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>5</v>
+      <c r="F2" s="0" t="n">
+        <f aca="false">RANK($D2, $D$2:$D$54, 0)</f>
+        <v>32</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,8 +542,12 @@
         <f aca="false">IF(D3=20,"A++",IF(D3&gt;=15,"A",IF(D3&gt;=12,"B",IF(D3&gt;=8,"C",IF(D3&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>6</v>
+      <c r="F3" s="0" t="n">
+        <f aca="false">RANK($D3, $D$2:$D$54, 0)</f>
+        <v>23</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,8 +559,12 @@
         <f aca="false">IF(D4=20,"A++",IF(D4&gt;=15,"A",IF(D4&gt;=12,"B",IF(D4&gt;=8,"C",IF(D4&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>7</v>
+      <c r="F4" s="0" t="e">
+        <f aca="false">RANK($D4, $D$2:$D$54, 0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,8 +578,12 @@
         <f aca="false">IF(D5=20,"A++",IF(D5&gt;=15,"A",IF(D5&gt;=12,"B",IF(D5&gt;=8,"C",IF(D5&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>8</v>
+      <c r="F5" s="0" t="n">
+        <f aca="false">RANK($D5, $D$2:$D$54, 0)</f>
+        <v>43</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,8 +597,12 @@
         <f aca="false">IF(D6=20,"A++",IF(D6&gt;=15,"A",IF(D6&gt;=12,"B",IF(D6&gt;=8,"C",IF(D6&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>9</v>
+      <c r="F6" s="0" t="n">
+        <f aca="false">RANK($D6, $D$2:$D$54, 0)</f>
+        <v>7</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,20 +616,28 @@
         <f aca="false">IF(D7=20,"A++",IF(D7&gt;=15,"A",IF(D7&gt;=12,"B",IF(D7&gt;=8,"C",IF(D7&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>10</v>
+      <c r="F7" s="0" t="n">
+        <f aca="false">RANK($D7, $D$2:$D$54, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="str">
         <f aca="false">IF(D8=20,"A++",IF(D8&gt;=15,"A",IF(D8&gt;=12,"B",IF(D8&gt;=8,"C",IF(D8&gt;=6,"D","E")))))</f>
         <v>E</v>
+      </c>
+      <c r="F8" s="0" t="e">
+        <f aca="false">RANK($D8, $D$2:$D$54, 0)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,6 +651,10 @@
         <f aca="false">IF(D9=20,"A++",IF(D9&gt;=15,"A",IF(D9&gt;=12,"B",IF(D9&gt;=8,"C",IF(D9&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">RANK($D9, $D$2:$D$54, 0)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
@@ -624,6 +667,10 @@
         <f aca="false">IF(D10=20,"A++",IF(D10&gt;=15,"A",IF(D10&gt;=12,"B",IF(D10&gt;=8,"C",IF(D10&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">RANK($D10, $D$2:$D$54, 0)</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
@@ -636,6 +683,10 @@
         <f aca="false">IF(D11=20,"A++",IF(D11&gt;=15,"A",IF(D11&gt;=12,"B",IF(D11&gt;=8,"C",IF(D11&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">RANK($D11, $D$2:$D$54, 0)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
@@ -648,6 +699,10 @@
         <f aca="false">IF(D12=20,"A++",IF(D12&gt;=15,"A",IF(D12&gt;=12,"B",IF(D12&gt;=8,"C",IF(D12&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <f aca="false">RANK($D12, $D$2:$D$54, 0)</f>
+        <v>27</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
@@ -660,6 +715,10 @@
         <f aca="false">IF(D13=20,"A++",IF(D13&gt;=15,"A",IF(D13&gt;=12,"B",IF(D13&gt;=8,"C",IF(D13&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <f aca="false">RANK($D13, $D$2:$D$54, 0)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
@@ -672,6 +731,10 @@
         <f aca="false">IF(D14=20,"A++",IF(D14&gt;=15,"A",IF(D14&gt;=12,"B",IF(D14&gt;=8,"C",IF(D14&gt;=6,"D","E")))))</f>
         <v>C</v>
       </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">RANK($D14, $D$2:$D$54, 0)</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
@@ -684,6 +747,10 @@
         <f aca="false">IF(D15=20,"A++",IF(D15&gt;=15,"A",IF(D15&gt;=12,"B",IF(D15&gt;=8,"C",IF(D15&gt;=6,"D","E")))))</f>
         <v>C</v>
       </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">RANK($D15, $D$2:$D$54, 0)</f>
+        <v>36</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
@@ -696,6 +763,10 @@
         <f aca="false">IF(D16=20,"A++",IF(D16&gt;=15,"A",IF(D16&gt;=12,"B",IF(D16&gt;=8,"C",IF(D16&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F16" s="0" t="n">
+        <f aca="false">RANK($D16, $D$2:$D$54, 0)</f>
+        <v>23</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
@@ -708,6 +779,10 @@
         <f aca="false">IF(D17=20,"A++",IF(D17&gt;=15,"A",IF(D17&gt;=12,"B",IF(D17&gt;=8,"C",IF(D17&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F17" s="0" t="n">
+        <f aca="false">RANK($D17, $D$2:$D$54, 0)</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
@@ -720,17 +795,25 @@
         <f aca="false">IF(D18=20,"A++",IF(D18&gt;=15,"A",IF(D18&gt;=12,"B",IF(D18&gt;=8,"C",IF(D18&gt;=6,"D","E")))))</f>
         <v>C</v>
       </c>
+      <c r="F18" s="0" t="n">
+        <f aca="false">RANK($D18, $D$2:$D$54, 0)</f>
+        <v>33</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="str">
         <f aca="false">IF(D19=20,"A++",IF(D19&gt;=15,"A",IF(D19&gt;=12,"B",IF(D19&gt;=8,"C",IF(D19&gt;=6,"D","E")))))</f>
         <v>E</v>
+      </c>
+      <c r="F19" s="0" t="e">
+        <f aca="false">RANK($D19, $D$2:$D$54, 0)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,6 +827,10 @@
         <f aca="false">IF(D20=20,"A++",IF(D20&gt;=15,"A",IF(D20&gt;=12,"B",IF(D20&gt;=8,"C",IF(D20&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
+      <c r="F20" s="0" t="n">
+        <f aca="false">RANK($D20, $D$2:$D$54, 0)</f>
+        <v>42</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
@@ -756,6 +843,10 @@
         <f aca="false">IF(D21=20,"A++",IF(D21&gt;=15,"A",IF(D21&gt;=12,"B",IF(D21&gt;=8,"C",IF(D21&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
+      <c r="F21" s="0" t="n">
+        <f aca="false">RANK($D21, $D$2:$D$54, 0)</f>
+        <v>43</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
@@ -768,6 +859,10 @@
         <f aca="false">IF(D22=20,"A++",IF(D22&gt;=15,"A",IF(D22&gt;=12,"B",IF(D22&gt;=8,"C",IF(D22&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">RANK($D22, $D$2:$D$54, 0)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
@@ -780,6 +875,10 @@
         <f aca="false">IF(D23=20,"A++",IF(D23&gt;=15,"A",IF(D23&gt;=12,"B",IF(D23&gt;=8,"C",IF(D23&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F23" s="0" t="n">
+        <f aca="false">RANK($D23, $D$2:$D$54, 0)</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
@@ -792,6 +891,10 @@
         <f aca="false">IF(D24=20,"A++",IF(D24&gt;=15,"A",IF(D24&gt;=12,"B",IF(D24&gt;=8,"C",IF(D24&gt;=6,"D","E")))))</f>
         <v>D</v>
       </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">RANK($D24, $D$2:$D$54, 0)</f>
+        <v>39</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
@@ -804,6 +907,10 @@
         <f aca="false">IF(D25=20,"A++",IF(D25&gt;=15,"A",IF(D25&gt;=12,"B",IF(D25&gt;=8,"C",IF(D25&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">RANK($D25, $D$2:$D$54, 0)</f>
+        <v>45</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7"/>
@@ -816,6 +923,10 @@
         <f aca="false">IF(D26=20,"A++",IF(D26&gt;=15,"A",IF(D26&gt;=12,"B",IF(D26&gt;=8,"C",IF(D26&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">RANK($D26, $D$2:$D$54, 0)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7"/>
@@ -828,6 +939,10 @@
         <f aca="false">IF(D27=20,"A++",IF(D27&gt;=15,"A",IF(D27&gt;=12,"B",IF(D27&gt;=8,"C",IF(D27&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F27" s="0" t="n">
+        <f aca="false">RANK($D27, $D$2:$D$54, 0)</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
@@ -840,6 +955,10 @@
         <f aca="false">IF(D28=20,"A++",IF(D28&gt;=15,"A",IF(D28&gt;=12,"B",IF(D28&gt;=8,"C",IF(D28&gt;=6,"D","E")))))</f>
         <v>C</v>
       </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">RANK($D28, $D$2:$D$54, 0)</f>
+        <v>35</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7"/>
@@ -852,6 +971,10 @@
         <f aca="false">IF(D29=20,"A++",IF(D29&gt;=15,"A",IF(D29&gt;=12,"B",IF(D29&gt;=8,"C",IF(D29&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">RANK($D29, $D$2:$D$54, 0)</f>
+        <v>46</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
@@ -864,6 +987,10 @@
         <f aca="false">IF(D30=20,"A++",IF(D30&gt;=15,"A",IF(D30&gt;=12,"B",IF(D30&gt;=8,"C",IF(D30&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F30" s="0" t="n">
+        <f aca="false">RANK($D30, $D$2:$D$54, 0)</f>
+        <v>27</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7"/>
@@ -876,6 +1003,10 @@
         <f aca="false">IF(D31=20,"A++",IF(D31&gt;=15,"A",IF(D31&gt;=12,"B",IF(D31&gt;=8,"C",IF(D31&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F31" s="0" t="n">
+        <f aca="false">RANK($D31, $D$2:$D$54, 0)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7"/>
@@ -888,6 +1019,10 @@
         <f aca="false">IF(D32=20,"A++",IF(D32&gt;=15,"A",IF(D32&gt;=12,"B",IF(D32&gt;=8,"C",IF(D32&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F32" s="0" t="n">
+        <f aca="false">RANK($D32, $D$2:$D$54, 0)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7"/>
@@ -900,6 +1035,10 @@
         <f aca="false">IF(D33=20,"A++",IF(D33&gt;=15,"A",IF(D33&gt;=12,"B",IF(D33&gt;=8,"C",IF(D33&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F33" s="0" t="n">
+        <f aca="false">RANK($D33, $D$2:$D$54, 0)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7"/>
@@ -912,6 +1051,10 @@
         <f aca="false">IF(D34=20,"A++",IF(D34&gt;=15,"A",IF(D34&gt;=12,"B",IF(D34&gt;=8,"C",IF(D34&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">RANK($D34, $D$2:$D$54, 0)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7"/>
@@ -924,6 +1067,10 @@
         <f aca="false">IF(D35=20,"A++",IF(D35&gt;=15,"A",IF(D35&gt;=12,"B",IF(D35&gt;=8,"C",IF(D35&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F35" s="0" t="n">
+        <f aca="false">RANK($D35, $D$2:$D$54, 0)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
@@ -936,6 +1083,10 @@
         <f aca="false">IF(D36=20,"A++",IF(D36&gt;=15,"A",IF(D36&gt;=12,"B",IF(D36&gt;=8,"C",IF(D36&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">RANK($D36, $D$2:$D$54, 0)</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7"/>
@@ -948,6 +1099,10 @@
         <f aca="false">IF(D37=20,"A++",IF(D37&gt;=15,"A",IF(D37&gt;=12,"B",IF(D37&gt;=8,"C",IF(D37&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F37" s="0" t="n">
+        <f aca="false">RANK($D37, $D$2:$D$54, 0)</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7"/>
@@ -960,6 +1115,10 @@
         <f aca="false">IF(D38=20,"A++",IF(D38&gt;=15,"A",IF(D38&gt;=12,"B",IF(D38&gt;=8,"C",IF(D38&gt;=6,"D","E")))))</f>
         <v>C</v>
       </c>
+      <c r="F38" s="0" t="n">
+        <f aca="false">RANK($D38, $D$2:$D$54, 0)</f>
+        <v>38</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7"/>
@@ -972,6 +1131,10 @@
         <f aca="false">IF(D39=20,"A++",IF(D39&gt;=15,"A",IF(D39&gt;=12,"B",IF(D39&gt;=8,"C",IF(D39&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
+      <c r="F39" s="0" t="n">
+        <f aca="false">RANK($D39, $D$2:$D$54, 0)</f>
+        <v>41</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7"/>
@@ -984,6 +1147,10 @@
         <f aca="false">IF(D40=20,"A++",IF(D40&gt;=15,"A",IF(D40&gt;=12,"B",IF(D40&gt;=8,"C",IF(D40&gt;=6,"D","E")))))</f>
         <v>C</v>
       </c>
+      <c r="F40" s="0" t="n">
+        <f aca="false">RANK($D40, $D$2:$D$54, 0)</f>
+        <v>31</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
@@ -995,6 +1162,10 @@
       <c r="E41" s="9" t="str">
         <f aca="false">IF(D41=20,"A++",IF(D41&gt;=15,"A",IF(D41&gt;=12,"B",IF(D41&gt;=8,"C",IF(D41&gt;=6,"D","E")))))</f>
         <v>C</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <f aca="false">RANK($D41, $D$2:$D$54, 0)</f>
+        <v>37</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,6 +1177,10 @@
         <f aca="false">IF(D42=20,"A++",IF(D42&gt;=15,"A",IF(D42&gt;=12,"B",IF(D42&gt;=8,"C",IF(D42&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
+      <c r="F42" s="0" t="e">
+        <f aca="false">RANK($D42, $D$2:$D$54, 0)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7"/>
@@ -1017,6 +1192,10 @@
       <c r="E43" s="9" t="str">
         <f aca="false">IF(D43=20,"A++",IF(D43&gt;=15,"A",IF(D43&gt;=12,"B",IF(D43&gt;=8,"C",IF(D43&gt;=6,"D","E")))))</f>
         <v>A++</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <f aca="false">RANK($D43, $D$2:$D$54, 0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,6 +1207,10 @@
         <f aca="false">IF(D44=20,"A++",IF(D44&gt;=15,"A",IF(D44&gt;=12,"B",IF(D44&gt;=8,"C",IF(D44&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
+      <c r="F44" s="0" t="e">
+        <f aca="false">RANK($D44, $D$2:$D$54, 0)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7"/>
@@ -1040,6 +1223,10 @@
         <f aca="false">IF(D45=20,"A++",IF(D45&gt;=15,"A",IF(D45&gt;=12,"B",IF(D45&gt;=8,"C",IF(D45&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F45" s="0" t="n">
+        <f aca="false">RANK($D45, $D$2:$D$54, 0)</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7"/>
@@ -1052,6 +1239,10 @@
         <f aca="false">IF(D46=20,"A++",IF(D46&gt;=15,"A",IF(D46&gt;=12,"B",IF(D46&gt;=8,"C",IF(D46&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F46" s="0" t="n">
+        <f aca="false">RANK($D46, $D$2:$D$54, 0)</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7"/>
@@ -1064,6 +1255,10 @@
         <f aca="false">IF(D47=20,"A++",IF(D47&gt;=15,"A",IF(D47&gt;=12,"B",IF(D47&gt;=8,"C",IF(D47&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F47" s="0" t="n">
+        <f aca="false">RANK($D47, $D$2:$D$54, 0)</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7"/>
@@ -1076,6 +1271,10 @@
         <f aca="false">IF(D48=20,"A++",IF(D48&gt;=15,"A",IF(D48&gt;=12,"B",IF(D48&gt;=8,"C",IF(D48&gt;=6,"D","E")))))</f>
         <v>D</v>
       </c>
+      <c r="F48" s="0" t="n">
+        <f aca="false">RANK($D48, $D$2:$D$54, 0)</f>
+        <v>40</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7"/>
@@ -1088,6 +1287,10 @@
         <f aca="false">IF(D49=20,"A++",IF(D49&gt;=15,"A",IF(D49&gt;=12,"B",IF(D49&gt;=8,"C",IF(D49&gt;=6,"D","E")))))</f>
         <v>C</v>
       </c>
+      <c r="F49" s="0" t="n">
+        <f aca="false">RANK($D49, $D$2:$D$54, 0)</f>
+        <v>34</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7"/>
@@ -1100,6 +1303,10 @@
         <f aca="false">IF(D50=20,"A++",IF(D50&gt;=15,"A",IF(D50&gt;=12,"B",IF(D50&gt;=8,"C",IF(D50&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
+      <c r="F50" s="0" t="n">
+        <f aca="false">RANK($D50, $D$2:$D$54, 0)</f>
+        <v>46</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7"/>
@@ -1112,6 +1319,10 @@
         <f aca="false">IF(D51=20,"A++",IF(D51&gt;=15,"A",IF(D51&gt;=12,"B",IF(D51&gt;=8,"C",IF(D51&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F51" s="0" t="n">
+        <f aca="false">RANK($D51, $D$2:$D$54, 0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7"/>
@@ -1124,6 +1335,10 @@
         <f aca="false">IF(D52=20,"A++",IF(D52&gt;=15,"A",IF(D52&gt;=12,"B",IF(D52&gt;=8,"C",IF(D52&gt;=6,"D","E")))))</f>
         <v>E</v>
       </c>
+      <c r="F52" s="0" t="n">
+        <f aca="false">RANK($D52, $D$2:$D$54, 0)</f>
+        <v>48</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7"/>
@@ -1136,6 +1351,10 @@
         <f aca="false">IF(D53=20,"A++",IF(D53&gt;=15,"A",IF(D53&gt;=12,"B",IF(D53&gt;=8,"C",IF(D53&gt;=6,"D","E")))))</f>
         <v>B</v>
       </c>
+      <c r="F53" s="0" t="n">
+        <f aca="false">RANK($D53, $D$2:$D$54, 0)</f>
+        <v>23</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
@@ -1148,6 +1367,10 @@
         <f aca="false">IF(D54=20,"A++",IF(D54&gt;=15,"A",IF(D54&gt;=12,"B",IF(D54&gt;=8,"C",IF(D54&gt;=6,"D","E")))))</f>
         <v>A</v>
       </c>
+      <c r="F54" s="0" t="n">
+        <f aca="false">RANK($D54, $D$2:$D$54, 0)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7"/>
@@ -1158,7 +1381,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D57" s="2" t="n">
         <f aca="false">SUM(D2:D55) / COUNT(D2:D55)</f>
@@ -1167,7 +1390,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D58" s="2" t="n">
         <f aca="false">MEDIAN(D2:D55)</f>
@@ -1176,7 +1399,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D59" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(D2:D55)</f>
@@ -1185,7 +1408,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D60" s="12" t="n">
         <f aca="false">(D59 / D57) * 100</f>
@@ -1195,7 +1418,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D61" s="2" t="n">
         <f aca="false">MIN(D2:D55)</f>
@@ -1204,7 +1427,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D62" s="2" t="n">
         <f aca="false">MAX(D2:D55)</f>
@@ -1213,7 +1436,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D63" s="13" t="n">
         <f aca="false">COUNTIF(D2:D55, "&gt;=15")</f>
@@ -1223,7 +1446,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D64" s="13" t="n">
         <f aca="false">COUNTIF(D2:D55, "&gt;=10")</f>
@@ -1233,7 +1456,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D65" s="14" t="n">
         <f aca="false">COUNTIF(D2:D55, "&lt;10")</f>
@@ -1243,7 +1466,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D66" s="2" t="n">
         <f aca="false">COUNTIF(D2:D55, "&lt;6")</f>
@@ -1251,57 +1474,83 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D67" s="16" t="n">
+      <c r="C67" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="2" t="n">
+        <f aca="false">COUNTIF(D2:D55, "&lt;=0")</f>
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="n">
+        <f aca="false">COUNTIF(E2:E55, "&lt;=0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" s="16" t="n">
         <f aca="false">COUNT(D2:D55)</f>
         <v>48</v>
       </c>
-      <c r="E67" s="16"/>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D68" s="17" t="n">
-        <f aca="false">(INT(ROUNDUP(D63/D67 * 100,2)))</f>
-        <v>33</v>
-      </c>
-      <c r="E68" s="17"/>
+      <c r="E68" s="16"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D69" s="17" t="n">
-        <f aca="false">(INT(ROUNDUP(D64/D67 * 100,2)))</f>
+        <f aca="false">(INT(ROUNDUP(D63/D68 * 100,2)))</f>
+        <v>33</v>
+      </c>
+      <c r="E69" s="17"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70" s="17" t="n">
+        <f aca="false">(INT(ROUNDUP(D64/D68 * 100,2)))</f>
         <v>72</v>
-      </c>
-      <c r="E69" s="17"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D70" s="17" t="n">
-        <f aca="false">(INT(ROUNDUP(D65/D67 * 100,2)))</f>
-        <v>27</v>
       </c>
       <c r="E70" s="17"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D71" s="17" t="n">
-        <f aca="false">(INT(ROUNDUP(D66/D67 * 100,2)))</f>
+        <f aca="false">(INT(ROUNDUP(D65/D68 * 100,2)))</f>
+        <v>27</v>
+      </c>
+      <c r="E71" s="17"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D72" s="17" t="n">
+        <f aca="false">(INT(ROUNDUP(D66/D68 * 100,2)))</f>
         <v>16</v>
       </c>
-      <c r="E71" s="17"/>
+      <c r="E72" s="17"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D73" s="17" t="n">
+        <f aca="false">(INT(ROUNDUP(D67/D68 * 100,2)))</f>
+        <v>0</v>
+      </c>
+      <c r="E73" s="17" t="e">
+        <f aca="false">(INT(ROUNDUP(E67/E68 * 100,2)))</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D66:E1048576 D1:E62">
+  <conditionalFormatting sqref="D1:E62 F1 D66:E1048576">
     <cfRule type="cellIs" priority="2" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>6</formula>
     </cfRule>

</xml_diff>